<commit_message>
replaced RPD with Revenue/Downloads
</commit_message>
<xml_diff>
--- a/Data_GamesCompanies/Data_2210.xlsx
+++ b/Data_GamesCompanies/Data_2210.xlsx
@@ -37,7 +37,7 @@
     <t>Cumulative Revenue</t>
   </si>
   <si>
-    <t>RPD As of Oct 31, 2022</t>
+    <t>Revenue/Downloads</t>
   </si>
   <si>
     <t>Paid Downloads</t>
@@ -1612,7 +1612,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1676,19 +1676,19 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2035,7 +2035,7 @@
     <col min="25" max="25" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>152</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>170</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="4">
         <v>26</v>
       </c>

</xml_diff>